<commit_message>
differentiate between participant and thermal notifiers
</commit_message>
<xml_diff>
--- a/src/test/resources/edu/ie3/util/scala/io/flexSignal.xlsx
+++ b/src/test/resources/edu/ie3/util/scala/io/flexSignal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriskittl/workspaces/simona/src/test/resources/edu/ie3/util/scala/io/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/IdeaProjects/simona/src/test/resources/edu/ie3/util/scala/io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203DE5CD-F316-E94E-9E65-7B2AA7BF04BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E55F0F-55ED-974A-A4FE-47D6800E17BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="node0" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>time</t>
   </si>
@@ -65,15 +65,23 @@
   <si>
     <t>SIMONA_load</t>
   </si>
+  <si>
+    <t>totalResLoad</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,9 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -420,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2929"/>
+  <dimension ref="A1:K2929"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -440,7 +449,7 @@
     <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -471,8 +480,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44562</v>
       </c>
@@ -503,8 +515,11 @@
       <c r="J2">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44562.125</v>
       </c>
@@ -535,8 +550,11 @@
       <c r="J3">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44562.25</v>
       </c>
@@ -567,8 +585,11 @@
       <c r="J4">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44562.375</v>
       </c>
@@ -599,8 +620,11 @@
       <c r="J5">
         <v>19.399999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44562.5</v>
       </c>
@@ -631,8 +655,11 @@
       <c r="J6">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44562.625</v>
       </c>
@@ -663,8 +690,11 @@
       <c r="J7">
         <v>19.600000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44562.75</v>
       </c>
@@ -695,8 +725,11 @@
       <c r="J8">
         <v>19.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44562.875</v>
       </c>
@@ -727,26 +760,29 @@
       <c r="J9">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -9495,10 +9531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J2929"/>
+  <dimension ref="A1:K2929"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9515,7 +9551,7 @@
     <col min="10" max="10" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9546,8 +9582,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44562</v>
       </c>
@@ -9578,8 +9617,11 @@
       <c r="J2">
         <v>29.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44562.125</v>
       </c>
@@ -9610,8 +9652,11 @@
       <c r="J3">
         <v>29.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44562.25</v>
       </c>
@@ -9642,8 +9687,11 @@
       <c r="J4">
         <v>29.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44562.375</v>
       </c>
@@ -9674,8 +9722,11 @@
       <c r="J5">
         <v>29.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44562.5</v>
       </c>
@@ -9706,8 +9757,11 @@
       <c r="J6">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>44562.625</v>
       </c>
@@ -9738,8 +9792,11 @@
       <c r="J7">
         <v>29.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>27.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>44562.75</v>
       </c>
@@ -9770,8 +9827,11 @@
       <c r="J8">
         <v>29.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>27.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>44562.875</v>
       </c>
@@ -9802,26 +9862,29 @@
       <c r="J9">
         <v>29.8</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>27.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>